<commit_message>
Added Video File Name column
</commit_message>
<xml_diff>
--- a/Performer Data.xlsx
+++ b/Performer Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,138 +11,145 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
+    <t>Raag</t>
+  </si>
+  <si>
+    <t>Taal</t>
+  </si>
+  <si>
     <t>Composition</t>
   </si>
   <si>
-    <t>Raag</t>
-  </si>
-  <si>
-    <t>Taal</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Chirag Agarwal</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>Jago Mohan Pyare</t>
-  </si>
-  <si>
-    <t>Bhairav</t>
-  </si>
-  <si>
-    <t>Teental</t>
-  </si>
-  <si>
-    <t>I am student of Smt. Chandrima Misra and Pt. Dr. Nagraj Rao Havaldar since 3 years.</t>
+    <t>Video File Name</t>
+  </si>
+  <si>
+    <t>Divya Shenoy</t>
+  </si>
+  <si>
+    <t>Have been learning from Pt. Dr. Nagaraj Rao Havaldar and Shri Omkarnath Havaldar for the past 7 years.</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Multani</t>
+  </si>
+  <si>
+    <t>Teentaal</t>
+  </si>
+  <si>
+    <t>Kangana Mundariya Mori Re</t>
+  </si>
+  <si>
+    <t>Divya Shenoy_Bangalore.mp4</t>
+  </si>
+  <si>
+    <t>Janani Kulkarni Deshpande</t>
+  </si>
+  <si>
+    <t>Student of Pt. Dr. Nagaraj Rao Havaldar and Shri. Omkarnath Havaldar for the last 17 years.</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kangan Mundariya Mori </t>
+  </si>
+  <si>
+    <t>Janani Kulkarni Deshpande_Bengaluru.mp4</t>
   </si>
   <si>
     <t>Sameer Kulkarni</t>
   </si>
   <si>
-    <t>Bengaluru</t>
-  </si>
-  <si>
-    <t>Pal Pal Beetat Sagaro</t>
-  </si>
-  <si>
-    <t>Tilak Kamod</t>
-  </si>
-  <si>
-    <t>I am student of Pt. Omkarnath Havaldar since 15 years. I will be presenting a composition by my Guruji.</t>
-  </si>
-  <si>
-    <t>Kailasnadh Komara</t>
-  </si>
-  <si>
-    <t>Hyderabad</t>
-  </si>
-  <si>
-    <t>Jiya Lage Na</t>
-  </si>
-  <si>
-    <t>Bihag</t>
-  </si>
-  <si>
-    <t>I am student of Pt. Omkarnath Havaldar since 5 years.</t>
-  </si>
-  <si>
-    <t>Rajaneesh Ananje</t>
-  </si>
-  <si>
-    <t>Aaj More Ghar Aaye</t>
-  </si>
-  <si>
-    <t>Kalavati</t>
-  </si>
-  <si>
-    <t>I am student of Pt. Dr. Nagraj Rao Havaldar since 7 years.</t>
-  </si>
-  <si>
-    <t>Tejaswini Niranjana</t>
-  </si>
-  <si>
-    <t>Paayal mori baaje jhanan jhanana</t>
-  </si>
-  <si>
-    <t>Nand</t>
-  </si>
-  <si>
-    <t>Sharva Bapat</t>
-  </si>
-  <si>
-    <t>Mana Mohan Murli Wala</t>
-  </si>
-  <si>
-    <t>Durga</t>
-  </si>
-  <si>
-    <t>I am student of Pt. Dr. Nagraj Rao Havaldar since 12 years.</t>
+    <t>Student of Pt. Dr. Nagaraj Rao Havaldar and Shri. Omkarnath Havaldar for the past 17 years.</t>
+  </si>
+  <si>
+    <t>Abhogi</t>
+  </si>
+  <si>
+    <t>Ektaal</t>
+  </si>
+  <si>
+    <t>Laaj Rakho Mori</t>
+  </si>
+  <si>
+    <t>Sameer Kulkarni_Bengaluru.mp4</t>
+  </si>
+  <si>
+    <t>V S Remya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student of Guruji Sri. Omkarnath Havaldar
+</t>
+  </si>
+  <si>
+    <t>Calicut</t>
+  </si>
+  <si>
+    <t>Gorakh Kalyan</t>
+  </si>
+  <si>
+    <t>Teen Taal</t>
+  </si>
+  <si>
+    <t>Baaje Murali</t>
+  </si>
+  <si>
+    <t>V S Remya_Calicut.mp4</t>
+  </si>
+  <si>
+    <t>Shreyas B Rao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This song is based on raag bhimpalasi set to taal teen taal. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BHIMPALASI </t>
+  </si>
+  <si>
+    <t>TEEN TAAL</t>
+  </si>
+  <si>
+    <t>JAARE APNE MANDIRVA</t>
+  </si>
+  <si>
+    <t>Shreyas-B-Rao_Bangalore.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-    </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,13 +162,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -376,13 +381,19 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.43"/>
-    <col customWidth="1" min="3" max="3" width="32.43"/>
-    <col customWidth="1" min="6" max="6" width="71.43"/>
+    <col customWidth="1" min="1" max="1" width="31.29"/>
+    <col customWidth="1" min="2" max="2" width="103.86"/>
+    <col customWidth="1" min="3" max="5" width="21.57"/>
+    <col customWidth="1" min="6" max="6" width="29.29"/>
+    <col customWidth="1" min="7" max="7" width="39.43"/>
+    <col customWidth="1" min="8" max="12" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -392,7 +403,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -404,125 +415,123 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>